<commit_message>
Dual number implemented / tested
</commit_message>
<xml_diff>
--- a/10_LogicPaper_math.xlsx
+++ b/10_LogicPaper_math.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\long_\git\jyborg\jyborg\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\long_\git\jyborg\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,9 +17,14 @@
     <sheet name="frac" sheetId="6" r:id="rId3"/>
     <sheet name="binarion" sheetId="9" r:id="rId4"/>
     <sheet name="dual" sheetId="10" r:id="rId5"/>
-    <sheet name="nm" sheetId="5" r:id="rId6"/>
-    <sheet name="quad" sheetId="7" r:id="rId7"/>
+    <sheet name="split" sheetId="12" r:id="rId6"/>
+    <sheet name="nm" sheetId="5" r:id="rId7"/>
+    <sheet name="quad" sheetId="7" r:id="rId8"/>
   </sheets>
+  <definedNames>
+    <definedName name="K" localSheetId="4">dual!$B$18</definedName>
+    <definedName name="X" localSheetId="4">dual!$C$18</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -30,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="188">
   <si>
     <t>Math</t>
     <phoneticPr fontId="3"/>
@@ -612,10 +617,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>f(x)=24</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>f1</t>
     <phoneticPr fontId="3"/>
   </si>
@@ -644,14 +645,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>f(x)=48</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>f(x)=x + 24</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>f(x)</t>
     <phoneticPr fontId="3"/>
   </si>
@@ -661,14 +654,6 @@
   </si>
   <si>
     <t>f(x)=2x</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>f(x)=24x</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>f(x)=576</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
@@ -684,15 +669,7 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>f(x)=-24</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>f(x)=-x</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>f(x)=1/24</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
@@ -704,15 +681,7 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>f(x)=1/(x+24)</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>f(x)=1/x/x</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>f(x)=24x^2</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
@@ -721,18 +690,6 @@
   </si>
   <si>
     <t>sqr</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>f(x)=24x^2</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>f(x)=1/x/x/24</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>f(x)=sqrt(x+24)</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
@@ -748,15 +705,7 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>f'(x)=-1/(x+24)^2</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>f'(x)=-/x^3</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>f'(x)=-/x^3/24</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
@@ -792,19 +741,11 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>f'(x)=24</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>f'(x)=2x</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>f'(x)=3x^2</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>f(x)=48x</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
@@ -820,15 +761,43 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>f(x)=2r6</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>f'(x)=1</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>f'(x)=1/2/sqrt(x+24)</t>
+    <t>Split Complex Numbers</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>~ silver / gold / dynamic rectangle grid points</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>a</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>b</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>nan</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>0 (default)</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>1 (unit)</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>c</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>test</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -1243,7 +1212,47 @@
     <cellStyle name="標準 2" xfId="1"/>
     <cellStyle name="標準 2 2" xfId="3"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="28">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1523,7 +1532,6 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1739,11 +1747,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1787070576"/>
-        <c:axId val="-1787074384"/>
+        <c:axId val="1404274416"/>
+        <c:axId val="1404260816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1787070576"/>
+        <c:axId val="1404274416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1800,12 +1808,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1787074384"/>
+        <c:crossAx val="1404260816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1787074384"/>
+        <c:axId val="1404260816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1862,7 +1870,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1787070576"/>
+        <c:crossAx val="1404274416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1876,7 +1884,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3477,8 +3484,8 @@
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="630622" cy="219163"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="テキスト ボックス 1"/>
@@ -3552,7 +3559,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="テキスト ボックス 1"/>
@@ -3611,8 +3618,8 @@
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="507126" cy="219163"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="テキスト ボックス 2"/>
@@ -3686,7 +3693,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="テキスト ボックス 2"/>
@@ -3745,8 +3752,8 @@
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="630622" cy="219163"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="テキスト ボックス 3"/>
@@ -3820,7 +3827,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="テキスト ボックス 3"/>
@@ -3879,8 +3886,8 @@
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1825180" cy="219163"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="テキスト ボックス 4"/>
@@ -4019,7 +4026,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="テキスト ボックス 4"/>
@@ -4078,8 +4085,8 @@
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="828817" cy="219163"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="テキスト ボックス 5"/>
@@ -4160,7 +4167,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="テキスト ボックス 5"/>
@@ -4219,8 +4226,8 @@
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="854465" cy="219163"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="テキスト ボックス 6"/>
@@ -4307,7 +4314,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="テキスト ボックス 6"/>
@@ -4366,8 +4373,8 @@
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1146276" cy="219163"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="テキスト ボックス 7"/>
@@ -4460,7 +4467,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="テキスト ボックス 7"/>
@@ -4519,8 +4526,8 @@
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="997517" cy="219163"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="テキスト ボックス 8"/>
@@ -4613,7 +4620,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="テキスト ボックス 8"/>
@@ -4672,8 +4679,8 @@
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2041906" cy="219163"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="テキスト ボックス 9"/>
@@ -4813,7 +4820,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="テキスト ボックス 9"/>
@@ -4872,8 +4879,8 @@
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2025811" cy="219163"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="テキスト ボックス 10"/>
@@ -5013,7 +5020,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="テキスト ボックス 10"/>
@@ -5072,8 +5079,8 @@
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="174728" cy="219163"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="テキスト ボックス 11"/>
@@ -5130,7 +5137,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="テキスト ボックス 11"/>
@@ -9531,8 +9538,8 @@
       <xdr:rowOff>161192</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="305725" cy="219163"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="38" name="テキスト ボックス 37"/>
@@ -9595,7 +9602,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="38" name="テキスト ボックス 37"/>
@@ -9659,8 +9666,8 @@
       <xdr:rowOff>56406</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1137298" cy="446020"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="テキスト ボックス 1"/>
@@ -9804,7 +9811,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="テキスト ボックス 1"/>
@@ -9880,8 +9887,8 @@
       <xdr:rowOff>102577</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1341393" cy="442237"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="テキスト ボックス 2"/>
@@ -10019,7 +10026,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="テキスト ボックス 2"/>
@@ -10095,8 +10102,8 @@
       <xdr:rowOff>109904</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1235658" cy="442237"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="テキスト ボックス 3"/>
@@ -10240,7 +10247,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="テキスト ボックス 3"/>
@@ -10316,8 +10323,8 @@
       <xdr:rowOff>43962</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1248675" cy="433580"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="テキスト ボックス 5"/>
@@ -10455,7 +10462,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="テキスト ボックス 5"/>
@@ -10531,8 +10538,8 @@
       <xdr:rowOff>109903</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2887137" cy="745717"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="テキスト ボックス 7"/>
@@ -10989,7 +10996,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="テキスト ボックス 7"/>
@@ -11104,8 +11111,8 @@
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1235658" cy="442237"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="テキスト ボックス 2"/>
@@ -11408,7 +11415,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="テキスト ボックス 2"/>
@@ -11545,8 +11552,8 @@
       <xdr:rowOff>33702</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="491225" cy="438325"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="テキスト ボックス 3"/>
@@ -11635,7 +11642,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="テキスト ボックス 3"/>
@@ -11711,8 +11718,8 @@
       <xdr:rowOff>47626</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1368457" cy="429669"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="テキスト ボックス 4"/>
@@ -11748,6 +11755,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -11797,6 +11805,7 @@
               </a:endParaRPr>
             </a:p>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -11853,7 +11862,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="テキスト ボックス 4"/>
@@ -11934,8 +11943,8 @@
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1368457" cy="429669"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="テキスト ボックス 5"/>
@@ -11971,6 +11980,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -12020,6 +12030,7 @@
               </a:endParaRPr>
             </a:p>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -12076,7 +12087,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="テキスト ボックス 5"/>
@@ -12153,12 +12164,12 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="968727" cy="438325"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="テキスト ボックス 6"/>
@@ -12546,7 +12557,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="テキスト ボックス 6"/>
@@ -12677,12 +12688,12 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1322990" cy="438325"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="テキスト ボックス 7"/>
@@ -13180,7 +13191,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="テキスト ボックス 7"/>
@@ -13311,12 +13322,12 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="701602" cy="438325"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="テキスト ボックス 8"/>
@@ -13562,7 +13573,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="テキスト ボックス 8"/>
@@ -13693,12 +13704,12 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="739818" cy="900375"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="テキスト ボックス 9"/>
@@ -14079,7 +14090,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="テキスト ボックス 9"/>
@@ -14210,12 +14221,12 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>66</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="670375" cy="628249"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="テキスト ボックス 10"/>
@@ -14523,7 +14534,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="テキスト ボックス 10"/>
@@ -14654,6 +14665,787 @@
 </file>
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>490904</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>36634</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2035429" cy="441596"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="テキスト ボックス 1"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="490904" y="1084384"/>
+              <a:ext cx="2035429" cy="441596"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr/>
+              </a:pPr>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                        <a:ln>
+                          <a:noFill/>
+                        </a:ln>
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:uLnTx/>
+                        <a:uFillTx/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>𝑎</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                        <a:ln>
+                          <a:noFill/>
+                        </a:ln>
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:uLnTx/>
+                        <a:uFillTx/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>+</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                        <a:ln>
+                          <a:noFill/>
+                        </a:ln>
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:uLnTx/>
+                        <a:uFillTx/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>𝑏</m:t>
+                    </m:r>
+                    <m:rad>
+                      <m:radPr>
+                        <m:degHide m:val="on"/>
+                        <m:ctrlPr>
+                          <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                            <a:ln>
+                              <a:noFill/>
+                            </a:ln>
+                            <a:solidFill>
+                              <a:sysClr val="windowText" lastClr="000000"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:uLnTx/>
+                            <a:uFillTx/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:radPr>
+                      <m:deg/>
+                      <m:e>
+                        <m:r>
+                          <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                            <a:ln>
+                              <a:noFill/>
+                            </a:ln>
+                            <a:solidFill>
+                              <a:sysClr val="windowText" lastClr="000000"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:uLnTx/>
+                            <a:uFillTx/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝑟</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:rad>
+                  </m:oMath>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                        <a:ln>
+                          <a:noFill/>
+                        </a:ln>
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:uLnTx/>
+                        <a:uFillTx/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>𝑟</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                        <a:ln>
+                          <a:noFill/>
+                        </a:ln>
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:uLnTx/>
+                        <a:uFillTx/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>∈</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                        <a:ln>
+                          <a:noFill/>
+                        </a:ln>
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:uLnTx/>
+                        <a:uFillTx/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>ℕ</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                        <a:ln>
+                          <a:noFill/>
+                        </a:ln>
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:uLnTx/>
+                        <a:uFillTx/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>, ∄</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                        <a:ln>
+                          <a:noFill/>
+                        </a:ln>
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:uLnTx/>
+                        <a:uFillTx/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>𝑚</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                        <a:ln>
+                          <a:noFill/>
+                        </a:ln>
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:uLnTx/>
+                        <a:uFillTx/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>∈</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                        <a:ln>
+                          <a:noFill/>
+                        </a:ln>
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:uLnTx/>
+                        <a:uFillTx/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>ℕ</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                        <a:ln>
+                          <a:noFill/>
+                        </a:ln>
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:uLnTx/>
+                        <a:uFillTx/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t> </m:t>
+                    </m:r>
+                    <m:r>
+                      <m:rPr>
+                        <m:sty m:val="p"/>
+                      </m:rPr>
+                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                        <a:ln>
+                          <a:noFill/>
+                        </a:ln>
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:uLnTx/>
+                        <a:uFillTx/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>s</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                        <a:ln>
+                          <a:noFill/>
+                        </a:ln>
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:uLnTx/>
+                        <a:uFillTx/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>.</m:t>
+                    </m:r>
+                    <m:r>
+                      <m:rPr>
+                        <m:sty m:val="p"/>
+                      </m:rPr>
+                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                        <a:ln>
+                          <a:noFill/>
+                        </a:ln>
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:uLnTx/>
+                        <a:uFillTx/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>t</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                        <a:ln>
+                          <a:noFill/>
+                        </a:ln>
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:uLnTx/>
+                        <a:uFillTx/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>. </m:t>
+                    </m:r>
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                            <a:ln>
+                              <a:noFill/>
+                            </a:ln>
+                            <a:solidFill>
+                              <a:sysClr val="windowText" lastClr="000000"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:uLnTx/>
+                            <a:uFillTx/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                            <a:ln>
+                              <a:noFill/>
+                            </a:ln>
+                            <a:solidFill>
+                              <a:sysClr val="windowText" lastClr="000000"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:uLnTx/>
+                            <a:uFillTx/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝑚</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                            <a:ln>
+                              <a:noFill/>
+                            </a:ln>
+                            <a:solidFill>
+                              <a:sysClr val="windowText" lastClr="000000"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:uLnTx/>
+                            <a:uFillTx/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSup>
+                    <m:r>
+                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                        <a:ln>
+                          <a:noFill/>
+                        </a:ln>
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:uLnTx/>
+                        <a:uFillTx/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                        <a:ln>
+                          <a:noFill/>
+                        </a:ln>
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                        <a:effectLst/>
+                        <a:uLnTx/>
+                        <a:uFillTx/>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:rPr>
+                      <m:t>𝑟</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:uLnTx/>
+                <a:uFillTx/>
+                <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                <a:ea typeface="ＭＳ Ｐゴシック" panose="020B0600070205080204" pitchFamily="50" charset="-128"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="テキスト ボックス 1"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="490904" y="1084384"/>
+              <a:ext cx="2035429" cy="441596"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:uLnTx/>
+                  <a:uFillTx/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑎+𝑏√𝑟</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:uLnTx/>
+                  <a:uFillTx/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t/>
+              </a:r>
+              <a:br>
+                <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:uLnTx/>
+                  <a:uFillTx/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+              </a:br>
+              <a:r>
+                <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:uLnTx/>
+                  <a:uFillTx/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑟∈ℕ, </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:uLnTx/>
+                  <a:uFillTx/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>∄𝑚∈ℕ s.t. 𝑚^2=𝑟</a:t>
+              </a:r>
+              <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:uLnTx/>
+                <a:uFillTx/>
+                <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                <a:ea typeface="ＭＳ Ｐゴシック" panose="020B0600070205080204" pitchFamily="50" charset="-128"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>407378</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>33702</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="492827" cy="429669"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="テキスト ボックス 2"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2473570" y="1806817"/>
+              <a:ext cx="492827" cy="429669"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑎</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>∈</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>ℚ</m:t>
+                    </m:r>
+                  </m:oMath>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑏</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>∈</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>ℚ</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="テキスト ボックス 2"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2473570" y="1806817"/>
+              <a:ext cx="492827" cy="429669"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑎∈ℚ</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t/>
+              </a:r>
+              <a:br>
+                <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+              </a:br>
+              <a:r>
+                <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑏∈ℚ</a:t>
+              </a:r>
+              <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -16449,7 +17241,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -18530,7 +19322,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A64" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.4">
@@ -28455,50 +29247,50 @@
   </sheetData>
   <phoneticPr fontId="3"/>
   <conditionalFormatting sqref="F15:F20">
-    <cfRule type="cellIs" dxfId="21" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="11" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="12" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J27:J30">
-    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="9" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="10" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J36:J39">
-    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="7" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="8" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F46:F49">
-    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="5" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F58:F62">
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="3" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="4" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F78:F81">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -28513,7 +29305,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -28583,33 +29375,33 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P72"/>
+  <dimension ref="A1:P77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N73" sqref="N73"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H77" sqref="H77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="3" max="3" width="10.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="30" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" s="30" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="30" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="19.5" thickTop="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" ht="19.5" thickTop="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B7" s="23" t="s">
         <v>129</v>
       </c>
@@ -28617,7 +29409,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B8" s="20" t="s">
         <v>130</v>
       </c>
@@ -28625,1260 +29417,1432 @@
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B10" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B16" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="C16" s="23"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="B17" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="B18" s="3">
+        <v>16</v>
+      </c>
+      <c r="C18" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="B20" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C20" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="D16" s="23" t="s">
+      <c r="D20" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="23" t="s">
+      <c r="E20" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="F16" s="23" t="s">
+      <c r="F20" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="G16" s="23" t="s">
+      <c r="G20" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="H16" s="23" t="s">
+      <c r="H20" s="23" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="B17" s="23">
-        <v>1</v>
-      </c>
-      <c r="C17" s="31" t="s">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="B21" s="23">
+        <v>1</v>
+      </c>
+      <c r="C21" s="31" t="str">
+        <f>"f(x)="&amp;K</f>
+        <v>f(x)=16</v>
+      </c>
+      <c r="D21" s="23">
+        <f>X</f>
+        <v>9</v>
+      </c>
+      <c r="E21" s="23">
+        <v>24</v>
+      </c>
+      <c r="F21" s="23">
+        <v>0</v>
+      </c>
+      <c r="G21" s="3">
+        <v>16</v>
+      </c>
+      <c r="H21" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="B22" s="23">
+        <v>2</v>
+      </c>
+      <c r="C22" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="D22" s="23">
+        <f>X</f>
+        <v>9</v>
+      </c>
+      <c r="E22" s="23">
+        <v>42</v>
+      </c>
+      <c r="F22" s="23">
+        <v>1</v>
+      </c>
+      <c r="G22" s="3">
+        <f>D22</f>
+        <v>9</v>
+      </c>
+      <c r="H22" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="B28" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="C28" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="D17" s="23">
-        <v>42</v>
-      </c>
-      <c r="E17" s="23">
-        <v>24</v>
-      </c>
-      <c r="F17" s="23">
+      <c r="D28" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="E28" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="F28" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="G28" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="H28" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="I28" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="J28" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="K28" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="L28" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="M28" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="N28" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="O28" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="P28" s="20" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="B29" s="23">
+        <v>1</v>
+      </c>
+      <c r="C29" s="31" t="str">
+        <f>"f(x)="&amp;K</f>
+        <v>f(x)=16</v>
+      </c>
+      <c r="D29" s="31" t="str">
+        <f>"f(x)="&amp;K</f>
+        <v>f(x)=16</v>
+      </c>
+      <c r="E29" s="31" t="str">
+        <f>"f(x)="&amp;K*2</f>
+        <v>f(x)=32</v>
+      </c>
+      <c r="F29" s="31" t="s">
+        <v>169</v>
+      </c>
+      <c r="G29" s="23">
+        <f t="shared" ref="G29:G31" si="0">X</f>
+        <v>9</v>
+      </c>
+      <c r="H29" s="23">
+        <f>2*K</f>
+        <v>32</v>
+      </c>
+      <c r="I29" s="31">
         <v>0</v>
       </c>
-      <c r="G17" s="3">
-        <v>24</v>
-      </c>
-      <c r="H17" s="3">
+      <c r="J29" s="34">
+        <f t="array" ref="J29:K29">G21:H21</f>
+        <v>16</v>
+      </c>
+      <c r="K29" s="35">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="B18" s="23">
+      <c r="L29" s="34">
+        <f t="array" ref="L29:M29">G21:H21</f>
+        <v>16</v>
+      </c>
+      <c r="M29" s="35">
+        <v>0</v>
+      </c>
+      <c r="N29" s="3">
+        <f>J29+L29</f>
+        <v>32</v>
+      </c>
+      <c r="O29" s="3">
+        <f>K29+M29</f>
+        <v>0</v>
+      </c>
+      <c r="P29" s="3" t="b">
+        <f>AND(N29=H29,O29=I29)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="B30" s="23">
         <v>2</v>
       </c>
-      <c r="C18" s="32" t="s">
+      <c r="C30" s="32" t="s">
         <v>141</v>
       </c>
-      <c r="D18" s="23">
-        <v>42</v>
-      </c>
-      <c r="E18" s="23">
-        <v>42</v>
-      </c>
-      <c r="F18" s="23">
-        <v>1</v>
-      </c>
-      <c r="G18" s="3">
-        <v>42</v>
-      </c>
-      <c r="H18" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A20" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="B24" s="23" t="s">
+      <c r="D30" s="31" t="str">
+        <f>"f(x)="&amp;K</f>
+        <v>f(x)=16</v>
+      </c>
+      <c r="E30" s="31" t="str">
+        <f>"f(x)=x+"&amp;K</f>
+        <v>f(x)=x+16</v>
+      </c>
+      <c r="F30" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="G30" s="23">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="H30" s="23">
+        <f>X+K</f>
+        <v>25</v>
+      </c>
+      <c r="I30" s="31">
+        <v>1</v>
+      </c>
+      <c r="J30" s="6">
+        <f t="array" ref="J30:K30">G22:H22</f>
+        <v>9</v>
+      </c>
+      <c r="K30" s="4">
+        <v>1</v>
+      </c>
+      <c r="L30" s="10">
+        <f t="array" ref="L30:M30">G21:H21</f>
+        <v>16</v>
+      </c>
+      <c r="M30" s="3">
+        <v>0</v>
+      </c>
+      <c r="N30" s="3">
+        <f t="shared" ref="N30:N31" si="1">J30+L30</f>
+        <v>25</v>
+      </c>
+      <c r="O30" s="3">
+        <f t="shared" ref="O30:O31" si="2">K30+M30</f>
+        <v>1</v>
+      </c>
+      <c r="P30" s="3" t="b">
+        <f t="shared" ref="P30:P31" si="3">AND(N30=H30,O30=I30)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="B31" s="33">
+        <v>3</v>
+      </c>
+      <c r="C31" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="D31" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="E31" s="32" t="s">
+        <v>151</v>
+      </c>
+      <c r="F31" s="32" t="s">
+        <v>171</v>
+      </c>
+      <c r="G31" s="23">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="H31" s="33">
+        <f>X*2</f>
+        <v>18</v>
+      </c>
+      <c r="I31" s="33">
+        <v>2</v>
+      </c>
+      <c r="J31" s="3">
+        <f t="array" ref="J31:K31">G22:H22</f>
+        <v>9</v>
+      </c>
+      <c r="K31" s="3">
+        <v>1</v>
+      </c>
+      <c r="L31" s="3">
+        <f t="array" ref="L31:M31">G22:H22</f>
+        <v>9</v>
+      </c>
+      <c r="M31" s="3">
+        <v>1</v>
+      </c>
+      <c r="N31" s="3">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="O31" s="3">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="P31" s="3" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A33" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="C36" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="B38" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="C24" s="23" t="s">
+      <c r="C38" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="D38" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="D24" s="23" t="s">
+      <c r="E38" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="F38" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="G38" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="H38" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="I38" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="J38" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="E24" s="23" t="s">
+      <c r="K38" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="L38" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="M38" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="N38" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="O38" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="P38" s="20" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="B39" s="23">
+        <v>1</v>
+      </c>
+      <c r="C39" s="31" t="str">
+        <f>"f(x)="&amp;K</f>
+        <v>f(x)=16</v>
+      </c>
+      <c r="D39" s="31" t="str">
+        <f>"f(x)="&amp;K</f>
+        <v>f(x)=16</v>
+      </c>
+      <c r="E39" s="31" t="str">
+        <f>"f(x)="&amp;K*K</f>
+        <v>f(x)=256</v>
+      </c>
+      <c r="F39" s="31" t="s">
+        <v>172</v>
+      </c>
+      <c r="G39" s="23">
+        <f t="shared" ref="G39:G43" si="4">X</f>
+        <v>9</v>
+      </c>
+      <c r="H39" s="23">
+        <f>K*K</f>
+        <v>256</v>
+      </c>
+      <c r="I39" s="31">
+        <v>0</v>
+      </c>
+      <c r="J39" s="34">
+        <f t="array" ref="J39:K39">$G$21:$H$21</f>
+        <v>16</v>
+      </c>
+      <c r="K39" s="35">
+        <v>0</v>
+      </c>
+      <c r="L39" s="34">
+        <f t="array" ref="L39:M39">$G$21:$H$21</f>
+        <v>16</v>
+      </c>
+      <c r="M39" s="35">
+        <v>0</v>
+      </c>
+      <c r="N39" s="3">
+        <f>J39*L39</f>
+        <v>256</v>
+      </c>
+      <c r="O39" s="3">
+        <f>J39*M39+K39*L39</f>
+        <v>0</v>
+      </c>
+      <c r="P39" s="3" t="b">
+        <f>AND(N39=H39,O39=I39)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="B40" s="23">
+        <v>2</v>
+      </c>
+      <c r="C40" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="D40" s="31" t="str">
+        <f>"f(x)="&amp;K</f>
+        <v>f(x)=16</v>
+      </c>
+      <c r="E40" s="31" t="str">
+        <f>"f(x)="&amp;K&amp;"x"</f>
+        <v>f(x)=16x</v>
+      </c>
+      <c r="F40" s="31" t="str">
+        <f>"f'(x)="&amp;K</f>
+        <v>f'(x)=16</v>
+      </c>
+      <c r="G40" s="23">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="H40" s="23">
+        <f>K*X</f>
+        <v>144</v>
+      </c>
+      <c r="I40" s="31">
+        <f>K</f>
+        <v>16</v>
+      </c>
+      <c r="J40" s="6">
+        <f t="array" ref="J40:K40">$G$22:$H$22</f>
+        <v>9</v>
+      </c>
+      <c r="K40" s="4">
+        <v>1</v>
+      </c>
+      <c r="L40" s="34">
+        <f t="array" ref="L40:M40">$G$21:$H$21</f>
+        <v>16</v>
+      </c>
+      <c r="M40" s="35">
+        <v>0</v>
+      </c>
+      <c r="N40" s="3">
+        <f t="shared" ref="N40:N42" si="5">J40*L40</f>
+        <v>144</v>
+      </c>
+      <c r="O40" s="3">
+        <f t="shared" ref="O40:O42" si="6">J40*M40+K40*L40</f>
+        <v>16</v>
+      </c>
+      <c r="P40" s="3" t="b">
+        <f t="shared" ref="P40:P41" si="7">AND(N40=H40,O40=I40)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="B41" s="33">
+        <v>3</v>
+      </c>
+      <c r="C41" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="D41" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="E41" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="F41" s="32" t="s">
+        <v>173</v>
+      </c>
+      <c r="G41" s="23">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="H41" s="33">
+        <f>G41^2</f>
+        <v>81</v>
+      </c>
+      <c r="I41" s="33">
+        <f>2*G41</f>
+        <v>18</v>
+      </c>
+      <c r="J41" s="6">
+        <f t="array" ref="J41:K41">$G$22:$H$22</f>
+        <v>9</v>
+      </c>
+      <c r="K41" s="4">
+        <v>1</v>
+      </c>
+      <c r="L41" s="6">
+        <f t="array" ref="L41:M41">$G$22:$H$22</f>
+        <v>9</v>
+      </c>
+      <c r="M41" s="4">
+        <v>1</v>
+      </c>
+      <c r="N41" s="3">
+        <f t="shared" si="5"/>
+        <v>81</v>
+      </c>
+      <c r="O41" s="3">
+        <f t="shared" si="6"/>
+        <v>18</v>
+      </c>
+      <c r="P41" s="3" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="B42" s="33">
+        <v>4</v>
+      </c>
+      <c r="C42" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="D42" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="E42" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="F42" s="32" t="s">
+        <v>174</v>
+      </c>
+      <c r="G42" s="23">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="H42" s="33">
+        <f>G42^3</f>
+        <v>729</v>
+      </c>
+      <c r="I42" s="33">
+        <f>3*X^2</f>
+        <v>243</v>
+      </c>
+      <c r="J42" s="3">
+        <f t="array" ref="J42:K42">J41:K41</f>
+        <v>9</v>
+      </c>
+      <c r="K42" s="3">
+        <v>1</v>
+      </c>
+      <c r="L42" s="3">
+        <f t="array" ref="L42:M42">N41:O41</f>
+        <v>81</v>
+      </c>
+      <c r="M42" s="3">
+        <v>18</v>
+      </c>
+      <c r="N42" s="3">
+        <f t="shared" si="5"/>
+        <v>729</v>
+      </c>
+      <c r="O42" s="3">
+        <f t="shared" si="6"/>
+        <v>243</v>
+      </c>
+      <c r="P42" s="3" t="b">
+        <f t="shared" ref="P42" si="8">AND(N42=H42,O42=I42)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="B43" s="33">
+        <v>5</v>
+      </c>
+      <c r="C43" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="D43" s="31" t="str">
+        <f>"f(x)="&amp;K</f>
+        <v>f(x)=16</v>
+      </c>
+      <c r="E43" s="32" t="str">
+        <f>"f(x)="&amp;K&amp;"x^2"</f>
+        <v>f(x)=16x^2</v>
+      </c>
+      <c r="F43" s="32" t="str">
+        <f>"f'(x)="&amp;K*2&amp;"x"</f>
+        <v>f'(x)=32x</v>
+      </c>
+      <c r="G43" s="23">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="H43" s="33">
+        <f>K*X*X</f>
+        <v>1296</v>
+      </c>
+      <c r="I43" s="33">
+        <f>2*K*X</f>
+        <v>288</v>
+      </c>
+      <c r="J43" s="3">
+        <f t="array" ref="J43:K43">N41:O41</f>
+        <v>81</v>
+      </c>
+      <c r="K43" s="3">
+        <v>18</v>
+      </c>
+      <c r="L43" s="3">
+        <f t="array" ref="L43:M43">$G$21:$H$21</f>
+        <v>16</v>
+      </c>
+      <c r="M43" s="3">
+        <v>0</v>
+      </c>
+      <c r="N43" s="3">
+        <f t="shared" ref="N43" si="9">J43*L43</f>
+        <v>1296</v>
+      </c>
+      <c r="O43" s="3">
+        <f t="shared" ref="O43" si="10">J43*M43+K43*L43</f>
+        <v>288</v>
+      </c>
+      <c r="P43" s="3" t="b">
+        <f t="shared" ref="P43" si="11">AND(N43=H43,O43=I43)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A46" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B49" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="C49" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="D49" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="F24" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="G24" s="23" t="s">
+      <c r="E49" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="F49" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="H24" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="I24" s="23" t="s">
-        <v>153</v>
-      </c>
-      <c r="J24" s="23" t="s">
-        <v>145</v>
-      </c>
-      <c r="K24" s="23" t="s">
+      <c r="G49" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="H49" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="I49" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="J49" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="L24" s="23" t="s">
+      <c r="K49" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="L49" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="M49" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="M24" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="N24" s="23" t="s">
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B50" s="23">
+        <v>1</v>
+      </c>
+      <c r="C50" s="31" t="str">
+        <f>"f(x)="&amp;K</f>
+        <v>f(x)=16</v>
+      </c>
+      <c r="D50" s="31" t="str">
+        <f>"f(x)=-"&amp;K</f>
+        <v>f(x)=-16</v>
+      </c>
+      <c r="E50" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="F50" s="23">
+        <f t="shared" ref="F50:F51" si="12">X</f>
+        <v>9</v>
+      </c>
+      <c r="G50" s="23">
+        <f>-K</f>
+        <v>-16</v>
+      </c>
+      <c r="H50" s="23">
+        <v>0</v>
+      </c>
+      <c r="I50" s="3">
+        <f t="array" ref="I50:J50">$G$21:$H$21</f>
+        <v>16</v>
+      </c>
+      <c r="J50" s="3">
+        <v>0</v>
+      </c>
+      <c r="K50" s="3">
+        <f>-I50</f>
+        <v>-16</v>
+      </c>
+      <c r="L50" s="3">
+        <f>-J50</f>
+        <v>0</v>
+      </c>
+      <c r="M50" s="3" t="b">
+        <f>AND(K50=G50,L50=H50)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B51" s="23">
+        <v>2</v>
+      </c>
+      <c r="C51" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="D51" s="31" t="s">
+        <v>155</v>
+      </c>
+      <c r="E51" s="31" t="s">
+        <v>167</v>
+      </c>
+      <c r="F51" s="23">
+        <f t="shared" si="12"/>
+        <v>9</v>
+      </c>
+      <c r="G51" s="23">
+        <f>-X</f>
+        <v>-9</v>
+      </c>
+      <c r="H51" s="23">
+        <v>-1</v>
+      </c>
+      <c r="I51" s="3">
+        <f t="array" ref="I51:J51">$G$22:$H$22</f>
+        <v>9</v>
+      </c>
+      <c r="J51" s="3">
+        <v>1</v>
+      </c>
+      <c r="K51" s="3">
+        <f>-I51</f>
+        <v>-9</v>
+      </c>
+      <c r="L51" s="3">
+        <f>-J51</f>
+        <v>-1</v>
+      </c>
+      <c r="M51" s="3" t="b">
+        <f>AND(K51=G51,L51=H51)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A54" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B59" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="C59" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="D59" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="E59" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="F59" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="G59" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="H59" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="I59" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="J59" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="K59" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="L59" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="O24" s="23" t="s">
-        <v>149</v>
-      </c>
-      <c r="P24" s="20" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="B25" s="23">
-        <v>1</v>
-      </c>
-      <c r="C25" s="31" t="s">
-        <v>142</v>
-      </c>
-      <c r="D25" s="31" t="s">
-        <v>142</v>
-      </c>
-      <c r="E25" s="31" t="s">
-        <v>150</v>
-      </c>
-      <c r="F25" s="31" t="s">
-        <v>183</v>
-      </c>
-      <c r="G25" s="23">
-        <v>42</v>
-      </c>
-      <c r="H25" s="23">
-        <v>48</v>
-      </c>
-      <c r="I25" s="31">
+      <c r="M59" s="20" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B60" s="23">
+        <v>1</v>
+      </c>
+      <c r="C60" s="31" t="str">
+        <f>"f(x)="&amp;K</f>
+        <v>f(x)=16</v>
+      </c>
+      <c r="D60" s="31" t="str">
+        <f>"f(x)= 1/"&amp;K</f>
+        <v>f(x)= 1/16</v>
+      </c>
+      <c r="E60" s="31" t="s">
+        <v>162</v>
+      </c>
+      <c r="F60" s="23">
+        <f>$D$21</f>
+        <v>9</v>
+      </c>
+      <c r="G60" s="23">
+        <f>1/K</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="H60" s="23">
         <v>0</v>
       </c>
-      <c r="J25" s="34">
-        <f t="array" ref="J25:K25">G17:H17</f>
-        <v>24</v>
-      </c>
-      <c r="K25" s="35">
+      <c r="I60" s="3">
+        <f t="array" ref="I60:J60">$G$21:$H$21</f>
+        <v>16</v>
+      </c>
+      <c r="J60" s="3">
         <v>0</v>
-      </c>
-      <c r="L25" s="34">
-        <f t="array" ref="L25:M25">G17:H17</f>
-        <v>24</v>
-      </c>
-      <c r="M25" s="35">
-        <v>0</v>
-      </c>
-      <c r="N25" s="3">
-        <f>J25+L25</f>
-        <v>48</v>
-      </c>
-      <c r="O25" s="3">
-        <f>K25+M25</f>
-        <v>0</v>
-      </c>
-      <c r="P25" s="3" t="b">
-        <f>AND(N25=H25,O25=I25)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="B26" s="23">
-        <v>2</v>
-      </c>
-      <c r="C26" s="32" t="s">
-        <v>141</v>
-      </c>
-      <c r="D26" s="31" t="s">
-        <v>142</v>
-      </c>
-      <c r="E26" s="31" t="s">
-        <v>151</v>
-      </c>
-      <c r="F26" s="31" t="s">
-        <v>184</v>
-      </c>
-      <c r="G26" s="23">
-        <v>42</v>
-      </c>
-      <c r="H26" s="23">
-        <f>G26+24</f>
-        <v>66</v>
-      </c>
-      <c r="I26" s="31">
-        <v>1</v>
-      </c>
-      <c r="J26" s="6">
-        <f t="array" ref="J26:K26">G18:H18</f>
-        <v>42</v>
-      </c>
-      <c r="K26" s="4">
-        <v>1</v>
-      </c>
-      <c r="L26" s="10">
-        <f t="array" ref="L26:M26">G17:H17</f>
-        <v>24</v>
-      </c>
-      <c r="M26" s="3">
-        <v>0</v>
-      </c>
-      <c r="N26" s="3">
-        <f t="shared" ref="N26:N27" si="0">J26+L26</f>
-        <v>66</v>
-      </c>
-      <c r="O26" s="3">
-        <f t="shared" ref="O26:O27" si="1">K26+M26</f>
-        <v>1</v>
-      </c>
-      <c r="P26" s="3" t="b">
-        <f t="shared" ref="P26:P27" si="2">AND(N26=H26,O26=I26)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="B27" s="33">
-        <v>3</v>
-      </c>
-      <c r="C27" s="32" t="s">
-        <v>141</v>
-      </c>
-      <c r="D27" s="32" t="s">
-        <v>141</v>
-      </c>
-      <c r="E27" s="32" t="s">
-        <v>154</v>
-      </c>
-      <c r="F27" s="32" t="s">
-        <v>185</v>
-      </c>
-      <c r="G27" s="33">
-        <v>42</v>
-      </c>
-      <c r="H27" s="33">
-        <f>G27*2</f>
-        <v>84</v>
-      </c>
-      <c r="I27" s="33">
-        <v>2</v>
-      </c>
-      <c r="J27" s="3">
-        <f t="array" ref="J27:K27">G18:H18</f>
-        <v>42</v>
-      </c>
-      <c r="K27" s="3">
-        <v>1</v>
-      </c>
-      <c r="L27" s="3">
-        <f t="array" ref="L27:M27">G18:H18</f>
-        <v>42</v>
-      </c>
-      <c r="M27" s="3">
-        <v>1</v>
-      </c>
-      <c r="N27" s="3">
-        <f t="shared" si="0"/>
-        <v>84</v>
-      </c>
-      <c r="O27" s="3">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="P27" s="3" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A29" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="C32" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="B34" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="C34" s="23" t="s">
-        <v>143</v>
-      </c>
-      <c r="D34" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="E34" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="F34" s="23" t="s">
-        <v>179</v>
-      </c>
-      <c r="G34" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="H34" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="I34" s="23" t="s">
-        <v>153</v>
-      </c>
-      <c r="J34" s="23" t="s">
-        <v>145</v>
-      </c>
-      <c r="K34" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="L34" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="M34" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="N34" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="O34" s="23" t="s">
-        <v>149</v>
-      </c>
-      <c r="P34" s="20" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="B35" s="23">
-        <v>1</v>
-      </c>
-      <c r="C35" s="31" t="s">
-        <v>142</v>
-      </c>
-      <c r="D35" s="31" t="s">
-        <v>142</v>
-      </c>
-      <c r="E35" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="F35" s="31" t="s">
-        <v>186</v>
-      </c>
-      <c r="G35" s="23">
-        <v>42</v>
-      </c>
-      <c r="H35" s="23">
-        <v>576</v>
-      </c>
-      <c r="I35" s="31">
-        <v>0</v>
-      </c>
-      <c r="J35" s="34">
-        <f t="array" ref="J35:K35">$G$17:$H$17</f>
-        <v>24</v>
-      </c>
-      <c r="K35" s="35">
-        <v>0</v>
-      </c>
-      <c r="L35" s="34">
-        <f t="array" ref="L35:M35">$G$17:$H$17</f>
-        <v>24</v>
-      </c>
-      <c r="M35" s="35">
-        <v>0</v>
-      </c>
-      <c r="N35" s="3">
-        <f>J35*L35</f>
-        <v>576</v>
-      </c>
-      <c r="O35" s="3">
-        <f>J35*M35+K35*L35</f>
-        <v>0</v>
-      </c>
-      <c r="P35" s="3" t="b">
-        <f>AND(N35=H35,O35=I35)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="B36" s="23">
-        <v>2</v>
-      </c>
-      <c r="C36" s="32" t="s">
-        <v>141</v>
-      </c>
-      <c r="D36" s="31" t="s">
-        <v>142</v>
-      </c>
-      <c r="E36" s="31" t="s">
-        <v>155</v>
-      </c>
-      <c r="F36" s="31" t="s">
-        <v>187</v>
-      </c>
-      <c r="G36" s="23">
-        <v>42</v>
-      </c>
-      <c r="H36" s="23">
-        <f>24*G36</f>
-        <v>1008</v>
-      </c>
-      <c r="I36" s="31">
-        <v>24</v>
-      </c>
-      <c r="J36" s="6">
-        <f t="array" ref="J36:K36">$G$18:$H$18</f>
-        <v>42</v>
-      </c>
-      <c r="K36" s="4">
-        <v>1</v>
-      </c>
-      <c r="L36" s="34">
-        <f t="array" ref="L36:M36">$G$17:$H$17</f>
-        <v>24</v>
-      </c>
-      <c r="M36" s="35">
-        <v>0</v>
-      </c>
-      <c r="N36" s="3">
-        <f t="shared" ref="N36:N38" si="3">J36*L36</f>
-        <v>1008</v>
-      </c>
-      <c r="O36" s="3">
-        <f t="shared" ref="O36:O38" si="4">J36*M36+K36*L36</f>
-        <v>24</v>
-      </c>
-      <c r="P36" s="3" t="b">
-        <f t="shared" ref="P36:P37" si="5">AND(N36=H36,O36=I36)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="B37" s="33">
-        <v>3</v>
-      </c>
-      <c r="C37" s="32" t="s">
-        <v>141</v>
-      </c>
-      <c r="D37" s="32" t="s">
-        <v>141</v>
-      </c>
-      <c r="E37" s="32" t="s">
-        <v>157</v>
-      </c>
-      <c r="F37" s="32" t="s">
-        <v>188</v>
-      </c>
-      <c r="G37" s="33">
-        <v>42</v>
-      </c>
-      <c r="H37" s="33">
-        <f>G37^2</f>
-        <v>1764</v>
-      </c>
-      <c r="I37" s="33">
-        <f>2*G37</f>
-        <v>84</v>
-      </c>
-      <c r="J37" s="6">
-        <f t="array" ref="J37:K37">$G$18:$H$18</f>
-        <v>42</v>
-      </c>
-      <c r="K37" s="4">
-        <v>1</v>
-      </c>
-      <c r="L37" s="6">
-        <f t="array" ref="L37:M37">$G$18:$H$18</f>
-        <v>42</v>
-      </c>
-      <c r="M37" s="4">
-        <v>1</v>
-      </c>
-      <c r="N37" s="3">
-        <f t="shared" si="3"/>
-        <v>1764</v>
-      </c>
-      <c r="O37" s="3">
-        <f t="shared" si="4"/>
-        <v>84</v>
-      </c>
-      <c r="P37" s="3" t="b">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="B38" s="33">
-        <v>4</v>
-      </c>
-      <c r="C38" s="32" t="s">
-        <v>141</v>
-      </c>
-      <c r="D38" s="32" t="s">
-        <v>157</v>
-      </c>
-      <c r="E38" s="32" t="s">
-        <v>158</v>
-      </c>
-      <c r="F38" s="32" t="s">
-        <v>189</v>
-      </c>
-      <c r="G38" s="33">
-        <v>42</v>
-      </c>
-      <c r="H38" s="33">
-        <f>G38^3</f>
-        <v>74088</v>
-      </c>
-      <c r="I38" s="33">
-        <f>3*G38^2</f>
-        <v>5292</v>
-      </c>
-      <c r="J38" s="3">
-        <f t="array" ref="J38:K38">J37:K37</f>
-        <v>42</v>
-      </c>
-      <c r="K38" s="3">
-        <v>1</v>
-      </c>
-      <c r="L38" s="3">
-        <f t="array" ref="L38:M38">N37:O37</f>
-        <v>1764</v>
-      </c>
-      <c r="M38" s="3">
-        <v>84</v>
-      </c>
-      <c r="N38" s="3">
-        <f t="shared" si="3"/>
-        <v>74088</v>
-      </c>
-      <c r="O38" s="3">
-        <f t="shared" si="4"/>
-        <v>5292</v>
-      </c>
-      <c r="P38" s="3" t="b">
-        <f t="shared" ref="P38" si="6">AND(N38=H38,O38=I38)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="B39" s="33">
-        <v>5</v>
-      </c>
-      <c r="C39" s="32" t="s">
-        <v>157</v>
-      </c>
-      <c r="D39" s="31" t="s">
-        <v>142</v>
-      </c>
-      <c r="E39" s="32" t="s">
-        <v>167</v>
-      </c>
-      <c r="F39" s="32" t="s">
-        <v>190</v>
-      </c>
-      <c r="G39" s="33">
-        <v>42</v>
-      </c>
-      <c r="H39" s="33">
-        <f>24*G39^2</f>
-        <v>42336</v>
-      </c>
-      <c r="I39" s="33">
-        <f>2*24*G39</f>
-        <v>2016</v>
-      </c>
-      <c r="J39" s="3">
-        <f t="array" ref="J39:K39">N37:O37</f>
-        <v>1764</v>
-      </c>
-      <c r="K39" s="3">
-        <v>84</v>
-      </c>
-      <c r="L39" s="3">
-        <f t="array" ref="L39:M39">$G$17:$H$17</f>
-        <v>24</v>
-      </c>
-      <c r="M39" s="3">
-        <v>0</v>
-      </c>
-      <c r="N39" s="3">
-        <f t="shared" ref="N39" si="7">J39*L39</f>
-        <v>42336</v>
-      </c>
-      <c r="O39" s="3">
-        <f t="shared" ref="O39" si="8">J39*M39+K39*L39</f>
-        <v>2016</v>
-      </c>
-      <c r="P39" s="3" t="b">
-        <f t="shared" ref="P39" si="9">AND(N39=H39,O39=I39)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A42" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="B45" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="C45" s="23" t="s">
-        <v>143</v>
-      </c>
-      <c r="D45" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E45" s="23" t="s">
-        <v>179</v>
-      </c>
-      <c r="F45" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="G45" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="H45" s="23" t="s">
-        <v>153</v>
-      </c>
-      <c r="I45" s="23" t="s">
-        <v>145</v>
-      </c>
-      <c r="J45" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="K45" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="L45" s="23" t="s">
-        <v>149</v>
-      </c>
-      <c r="M45" s="20" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="B46" s="23">
-        <v>1</v>
-      </c>
-      <c r="C46" s="31" t="s">
-        <v>142</v>
-      </c>
-      <c r="D46" s="31" t="s">
-        <v>160</v>
-      </c>
-      <c r="E46" s="31" t="s">
-        <v>180</v>
-      </c>
-      <c r="F46" s="23">
-        <v>42</v>
-      </c>
-      <c r="G46" s="23">
-        <v>-24</v>
-      </c>
-      <c r="H46" s="23">
-        <v>0</v>
-      </c>
-      <c r="I46" s="3">
-        <f t="array" ref="I46:J46">$G$17:$H$17</f>
-        <v>24</v>
-      </c>
-      <c r="J46" s="3">
-        <v>0</v>
-      </c>
-      <c r="K46" s="3">
-        <f>-I46</f>
-        <v>-24</v>
-      </c>
-      <c r="L46" s="3">
-        <f>-J46</f>
-        <v>0</v>
-      </c>
-      <c r="M46" s="3" t="b">
-        <f>AND(K46=G46,L46=H46)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="B47" s="23">
-        <v>2</v>
-      </c>
-      <c r="C47" s="32" t="s">
-        <v>141</v>
-      </c>
-      <c r="D47" s="31" t="s">
-        <v>161</v>
-      </c>
-      <c r="E47" s="31" t="s">
-        <v>181</v>
-      </c>
-      <c r="F47" s="23">
-        <v>42</v>
-      </c>
-      <c r="G47" s="23">
-        <f>-F47</f>
-        <v>-42</v>
-      </c>
-      <c r="H47" s="23">
-        <v>-1</v>
-      </c>
-      <c r="I47" s="3">
-        <f t="array" ref="I47:J47">$G$18:$H$18</f>
-        <v>42</v>
-      </c>
-      <c r="J47" s="3">
-        <v>1</v>
-      </c>
-      <c r="K47" s="3">
-        <f>-I47</f>
-        <v>-42</v>
-      </c>
-      <c r="L47" s="3">
-        <f>-J47</f>
-        <v>-1</v>
-      </c>
-      <c r="M47" s="3" t="b">
-        <f>AND(K47=G47,L47=H47)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A50" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="B55" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="C55" s="23" t="s">
-        <v>143</v>
-      </c>
-      <c r="D55" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E55" s="23" t="s">
-        <v>179</v>
-      </c>
-      <c r="F55" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="G55" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="H55" s="23" t="s">
-        <v>153</v>
-      </c>
-      <c r="I55" s="23" t="s">
-        <v>145</v>
-      </c>
-      <c r="J55" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="K55" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="L55" s="23" t="s">
-        <v>149</v>
-      </c>
-      <c r="M55" s="20" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="B56" s="23">
-        <v>1</v>
-      </c>
-      <c r="C56" s="31" t="s">
-        <v>142</v>
-      </c>
-      <c r="D56" s="31" t="s">
-        <v>162</v>
-      </c>
-      <c r="E56" s="31" t="s">
-        <v>174</v>
-      </c>
-      <c r="F56" s="23">
-        <v>42</v>
-      </c>
-      <c r="G56" s="23">
-        <f>1/24</f>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="H56" s="23">
-        <v>0</v>
-      </c>
-      <c r="I56" s="3">
-        <f t="array" ref="I56:J56">$G$17:$H$17</f>
-        <v>24</v>
-      </c>
-      <c r="J56" s="3">
-        <v>0</v>
-      </c>
-      <c r="K56" s="3">
-        <f>1/I56</f>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="L56" s="3">
-        <f>-J56/I56/I56</f>
-        <v>0</v>
-      </c>
-      <c r="M56" s="3" t="b">
-        <f>AND(K56=G56,L56=H56)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="B57" s="23">
-        <v>2</v>
-      </c>
-      <c r="C57" s="32" t="s">
-        <v>141</v>
-      </c>
-      <c r="D57" s="31" t="s">
-        <v>163</v>
-      </c>
-      <c r="E57" s="31" t="s">
-        <v>175</v>
-      </c>
-      <c r="F57" s="23">
-        <v>42</v>
-      </c>
-      <c r="G57" s="23">
-        <f>1/F57</f>
-        <v>2.3809523809523808E-2</v>
-      </c>
-      <c r="H57" s="23">
-        <f>-1/F57/F57</f>
-        <v>-5.6689342403628119E-4</v>
-      </c>
-      <c r="I57" s="3">
-        <f t="array" ref="I57:J57">$G$18:$H$18</f>
-        <v>42</v>
-      </c>
-      <c r="J57" s="3">
-        <v>1</v>
-      </c>
-      <c r="K57" s="3">
-        <f>1/I57</f>
-        <v>2.3809523809523808E-2</v>
-      </c>
-      <c r="L57" s="3">
-        <f>-J57/I57/I57</f>
-        <v>-5.6689342403628119E-4</v>
-      </c>
-      <c r="M57" s="3" t="b">
-        <f>AND(K57=G57,L57=H57)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="B58" s="23">
-        <v>3</v>
-      </c>
-      <c r="C58" s="32" t="s">
-        <v>164</v>
-      </c>
-      <c r="D58" s="31" t="s">
-        <v>165</v>
-      </c>
-      <c r="E58" s="31" t="s">
-        <v>176</v>
-      </c>
-      <c r="F58" s="23">
-        <v>42</v>
-      </c>
-      <c r="G58" s="23">
-        <f>1/(F58+24)</f>
-        <v>1.5151515151515152E-2</v>
-      </c>
-      <c r="H58" s="23">
-        <f>-1/(F58+24)^2</f>
-        <v>-2.295684113865932E-4</v>
-      </c>
-      <c r="I58" s="3">
-        <f t="array" ref="I58:J58">N26:O26</f>
-        <v>66</v>
-      </c>
-      <c r="J58" s="3">
-        <v>1</v>
-      </c>
-      <c r="K58" s="3">
-        <f>1/I58</f>
-        <v>1.5151515151515152E-2</v>
-      </c>
-      <c r="L58" s="3">
-        <f>-J58/I58/I58</f>
-        <v>-2.295684113865932E-4</v>
-      </c>
-      <c r="M58" s="3" t="b">
-        <f>AND(K58=G58,L58=H58)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="B59" s="23">
-        <v>4</v>
-      </c>
-      <c r="C59" s="32" t="s">
-        <v>157</v>
-      </c>
-      <c r="D59" s="31" t="s">
-        <v>166</v>
-      </c>
-      <c r="E59" s="31" t="s">
-        <v>177</v>
-      </c>
-      <c r="F59" s="23">
-        <v>42</v>
-      </c>
-      <c r="G59" s="23">
-        <f>1/F59/F59</f>
-        <v>5.6689342403628119E-4</v>
-      </c>
-      <c r="H59" s="23">
-        <f>-2/F59/F59/F59</f>
-        <v>-2.6994924954108629E-5</v>
-      </c>
-      <c r="I59" s="3">
-        <f t="array" ref="I59:J59">N37:O37</f>
-        <v>1764</v>
-      </c>
-      <c r="J59" s="3">
-        <v>84</v>
-      </c>
-      <c r="K59" s="3">
-        <f>1/I59</f>
-        <v>5.6689342403628119E-4</v>
-      </c>
-      <c r="L59" s="3">
-        <f>-J59/I59/I59</f>
-        <v>-2.6994924954108625E-5</v>
-      </c>
-      <c r="M59" s="3" t="b">
-        <f>AND(K59=G59,L59=H59)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="B60" s="33">
-        <v>5</v>
-      </c>
-      <c r="C60" s="32" t="s">
-        <v>170</v>
-      </c>
-      <c r="D60" s="31" t="s">
-        <v>171</v>
-      </c>
-      <c r="E60" s="31" t="s">
-        <v>178</v>
-      </c>
-      <c r="F60" s="23">
-        <v>42</v>
-      </c>
-      <c r="G60" s="23">
-        <f>1/F60/F60/24</f>
-        <v>2.362055933484505E-5</v>
-      </c>
-      <c r="H60" s="23">
-        <f>-2/F60/F60/F60/24</f>
-        <v>-1.1247885397545262E-6</v>
-      </c>
-      <c r="I60" s="3">
-        <f t="array" ref="I60:J60">N39:O39</f>
-        <v>42336</v>
-      </c>
-      <c r="J60" s="3">
-        <v>2016</v>
       </c>
       <c r="K60" s="3">
         <f>1/I60</f>
-        <v>2.362055933484505E-5</v>
+        <v>6.25E-2</v>
       </c>
       <c r="L60" s="3">
         <f>-J60/I60/I60</f>
-        <v>-1.124788539754526E-6</v>
+        <v>0</v>
       </c>
       <c r="M60" s="3" t="b">
         <f>AND(K60=G60,L60=H60)</f>
         <v>1</v>
       </c>
     </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B61" s="23">
+        <v>2</v>
+      </c>
+      <c r="C61" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="D61" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="E61" s="31" t="s">
+        <v>163</v>
+      </c>
+      <c r="F61" s="23">
+        <f t="shared" ref="F61:F65" si="13">$D$21</f>
+        <v>9</v>
+      </c>
+      <c r="G61" s="23">
+        <f>1/X</f>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="H61" s="23">
+        <f>-1/X/X</f>
+        <v>-1.2345679012345678E-2</v>
+      </c>
+      <c r="I61" s="3">
+        <f t="array" ref="I61:J61">$G$22:$H$22</f>
+        <v>9</v>
+      </c>
+      <c r="J61" s="3">
+        <v>1</v>
+      </c>
+      <c r="K61" s="3">
+        <f>1/I61</f>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="L61" s="3">
+        <f>-J61/I61/I61</f>
+        <v>-1.2345679012345678E-2</v>
+      </c>
+      <c r="M61" s="3" t="b">
+        <f>AND(K61=G61,L61=H61)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B62" s="23">
+        <v>3</v>
+      </c>
+      <c r="C62" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="D62" s="31" t="str">
+        <f>"f(x)=1/(x+"&amp;K&amp;")"</f>
+        <v>f(x)=1/(x+16)</v>
+      </c>
+      <c r="E62" s="31" t="str">
+        <f>"f'(x)=-1/(x+"&amp;K&amp;")^2"</f>
+        <v>f'(x)=-1/(x+16)^2</v>
+      </c>
+      <c r="F62" s="23">
+        <f t="shared" si="13"/>
+        <v>9</v>
+      </c>
+      <c r="G62" s="23">
+        <f>1/(X+K)</f>
+        <v>0.04</v>
+      </c>
+      <c r="H62" s="23">
+        <f>-1/(X+K)^2</f>
+        <v>-1.6000000000000001E-3</v>
+      </c>
+      <c r="I62" s="3">
+        <f t="array" ref="I62:J62">N30:O30</f>
+        <v>25</v>
+      </c>
+      <c r="J62" s="3">
+        <v>1</v>
+      </c>
+      <c r="K62" s="3">
+        <f>1/I62</f>
+        <v>0.04</v>
+      </c>
+      <c r="L62" s="3">
+        <f>-J62/I62/I62</f>
+        <v>-1.6000000000000001E-3</v>
+      </c>
+      <c r="M62" s="3" t="b">
+        <f>AND(K62=G62,L62=H62)</f>
+        <v>1</v>
+      </c>
+    </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A63" t="s">
+      <c r="B63" s="23">
+        <v>4</v>
+      </c>
+      <c r="C63" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="D63" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="E63" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="F63" s="23">
+        <f t="shared" si="13"/>
+        <v>9</v>
+      </c>
+      <c r="G63" s="23">
+        <f>1/X/X</f>
+        <v>1.2345679012345678E-2</v>
+      </c>
+      <c r="H63" s="23">
+        <f>-2/X/X/X</f>
+        <v>-2.7434842249657062E-3</v>
+      </c>
+      <c r="I63" s="3">
+        <f t="array" ref="I63:J63">N41:O41</f>
+        <v>81</v>
+      </c>
+      <c r="J63" s="3">
+        <v>18</v>
+      </c>
+      <c r="K63" s="3">
+        <f>1/I63</f>
+        <v>1.2345679012345678E-2</v>
+      </c>
+      <c r="L63" s="3">
+        <f>-J63/I63/I63</f>
+        <v>-2.7434842249657062E-3</v>
+      </c>
+      <c r="M63" s="3" t="b">
+        <f>AND(K63=G63,L63=H63)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B64" s="33">
+        <v>5</v>
+      </c>
+      <c r="C64" s="32" t="str">
+        <f>"f(x)="&amp;K&amp;"x^2"</f>
+        <v>f(x)=16x^2</v>
+      </c>
+      <c r="D64" s="31" t="str">
+        <f>"f(x)=1/x/x/"&amp;K</f>
+        <v>f(x)=1/x/x/16</v>
+      </c>
+      <c r="E64" s="31" t="str">
+        <f>"f'(x)=-/x^3/"&amp;K</f>
+        <v>f'(x)=-/x^3/16</v>
+      </c>
+      <c r="F64" s="23">
+        <f t="shared" si="13"/>
+        <v>9</v>
+      </c>
+      <c r="G64" s="23">
+        <f>1/X/X/K</f>
+        <v>7.716049382716049E-4</v>
+      </c>
+      <c r="H64" s="23">
+        <f>-2/X/X/X/K</f>
+        <v>-1.7146776406035664E-4</v>
+      </c>
+      <c r="I64" s="3">
+        <f t="array" ref="I64:J64">N43:O43</f>
+        <v>1296</v>
+      </c>
+      <c r="J64" s="3">
+        <v>288</v>
+      </c>
+      <c r="K64" s="3">
+        <f>1/I64</f>
+        <v>7.716049382716049E-4</v>
+      </c>
+      <c r="L64" s="3">
+        <f>-J64/I64/I64</f>
+        <v>-1.7146776406035664E-4</v>
+      </c>
+      <c r="M64" s="3" t="b">
+        <f>AND(K64=G64,L64=H64)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B65" s="33">
+        <v>6</v>
+      </c>
+      <c r="C65" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="D65" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="E65" s="31" t="s">
+        <v>163</v>
+      </c>
+      <c r="F65" s="23">
+        <v>0</v>
+      </c>
+      <c r="G65" s="23" t="e">
+        <f>1/F65</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H65" s="23" t="e">
+        <f>-1/F65/F65</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I65" s="3">
+        <v>0</v>
+      </c>
+      <c r="J65" s="3">
+        <v>1</v>
+      </c>
+      <c r="K65" s="3" t="e">
+        <f>1/I65</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L65" s="3" t="e">
+        <f>-J65/I65/I65</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M65" s="3" t="e">
+        <f>AND(K65=G65,L65=H65)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A67" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B72" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="C72" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="D72" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="E72" s="23" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="68" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B68" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="C68" s="23" t="s">
-        <v>143</v>
-      </c>
-      <c r="D68" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="E68" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="F68" s="23" t="s">
+      <c r="F72" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="G68" s="23" t="s">
+      <c r="G72" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="H72" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="I72" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="J72" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="K72" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="L72" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="M72" s="20" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B73" s="23">
+        <v>1</v>
+      </c>
+      <c r="C73" s="31" t="str">
+        <f>"f(x)="&amp;K</f>
+        <v>f(x)=16</v>
+      </c>
+      <c r="D73" s="31" t="str">
+        <f>"f(x)="&amp;SQRT(K)</f>
+        <v>f(x)=4</v>
+      </c>
+      <c r="E73" s="31" t="s">
+        <v>175</v>
+      </c>
+      <c r="F73" s="23">
+        <f t="shared" ref="F73:F77" si="14">$D$21</f>
+        <v>9</v>
+      </c>
+      <c r="G73" s="23">
+        <f>SQRT(K)</f>
+        <v>4</v>
+      </c>
+      <c r="H73" s="23">
+        <v>0</v>
+      </c>
+      <c r="I73" s="3">
+        <f t="array" ref="I73:J73">$G$21:$H$21</f>
+        <v>16</v>
+      </c>
+      <c r="J73" s="3">
+        <v>0</v>
+      </c>
+      <c r="K73" s="3">
+        <f>SQRT(I73)</f>
+        <v>4</v>
+      </c>
+      <c r="L73" s="3">
+        <f>J73/2/K73</f>
+        <v>0</v>
+      </c>
+      <c r="M73" s="3" t="b">
+        <f>AND(K73=G73,L73=H73)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B74" s="23">
+        <v>2</v>
+      </c>
+      <c r="C74" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="D74" s="31" t="s">
+        <v>161</v>
+      </c>
+      <c r="E74" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="F74" s="23">
+        <f t="shared" si="14"/>
+        <v>9</v>
+      </c>
+      <c r="G74" s="23">
+        <f>SQRT(F74)</f>
+        <v>3</v>
+      </c>
+      <c r="H74" s="23">
+        <f>1/2/SQRT(X)</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I74" s="3">
+        <f t="array" ref="I74:J74">$G$22:$H$22</f>
+        <v>9</v>
+      </c>
+      <c r="J74" s="3">
+        <v>1</v>
+      </c>
+      <c r="K74" s="3">
+        <f t="shared" ref="K74:K76" si="15">SQRT(I74)</f>
+        <v>3</v>
+      </c>
+      <c r="L74" s="3">
+        <f t="shared" ref="L74:L76" si="16">J74/2/K74</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="M74" s="3" t="b">
+        <f>AND(K74=G74,L74=H74)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B75" s="23">
+        <v>3</v>
+      </c>
+      <c r="C75" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="D75" s="31" t="str">
+        <f>"f(x)=sqrt(x+"&amp;K&amp;")"</f>
+        <v>f(x)=sqrt(x+16)</v>
+      </c>
+      <c r="E75" s="31" t="str">
+        <f>"f'(x)=1/2/sqrt(x+"&amp;K&amp;")"</f>
+        <v>f'(x)=1/2/sqrt(x+16)</v>
+      </c>
+      <c r="F75" s="23">
+        <f t="shared" si="14"/>
+        <v>9</v>
+      </c>
+      <c r="G75" s="23">
+        <f>SQRT(X+K)</f>
+        <v>5</v>
+      </c>
+      <c r="H75" s="23">
+        <f>1/2/SQRT(X+K)</f>
+        <v>0.1</v>
+      </c>
+      <c r="I75" s="3">
+        <f t="array" ref="I75:J75">N30:$O$30</f>
+        <v>25</v>
+      </c>
+      <c r="J75" s="3">
+        <v>1</v>
+      </c>
+      <c r="K75" s="3">
+        <f t="shared" si="15"/>
+        <v>5</v>
+      </c>
+      <c r="L75" s="3">
+        <f t="shared" si="16"/>
+        <v>0.1</v>
+      </c>
+      <c r="M75" s="3" t="b">
+        <f>AND(K75=G75,L75=H75)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B76" s="23">
+        <v>4</v>
+      </c>
+      <c r="C76" s="32" t="s">
         <v>152</v>
       </c>
-      <c r="H68" s="23" t="s">
-        <v>153</v>
-      </c>
-      <c r="I68" s="23" t="s">
-        <v>145</v>
-      </c>
-      <c r="J68" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="K68" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="L68" s="23" t="s">
-        <v>149</v>
-      </c>
-      <c r="M68" s="20" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="69" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B69" s="23">
-        <v>1</v>
-      </c>
-      <c r="C69" s="31" t="s">
-        <v>142</v>
-      </c>
-      <c r="D69" s="31" t="s">
-        <v>194</v>
-      </c>
-      <c r="E69" s="31" t="s">
-        <v>191</v>
-      </c>
-      <c r="F69" s="23">
-        <v>42</v>
-      </c>
-      <c r="G69" s="23">
-        <f>2*SQRT(6)</f>
-        <v>4.8989794855663558</v>
-      </c>
-      <c r="H69" s="23">
-        <v>0</v>
-      </c>
-      <c r="I69" s="3">
-        <f t="array" ref="I69:J69">$G$17:$H$17</f>
-        <v>24</v>
-      </c>
-      <c r="J69" s="3">
-        <v>0</v>
-      </c>
-      <c r="K69" s="3">
-        <f>SQRT(I69)</f>
-        <v>4.8989794855663558</v>
-      </c>
-      <c r="L69" s="3">
-        <f>J69/2/K69</f>
-        <v>0</v>
-      </c>
-      <c r="M69" s="3" t="b">
-        <f>AND(K69=G69,L69=H69)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B70" s="23">
-        <v>2</v>
-      </c>
-      <c r="C70" s="32" t="s">
+      <c r="D76" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="E76" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="F76" s="23">
+        <f t="shared" si="14"/>
+        <v>9</v>
+      </c>
+      <c r="G76" s="23">
+        <f>X</f>
+        <v>9</v>
+      </c>
+      <c r="H76" s="23">
+        <v>1</v>
+      </c>
+      <c r="I76" s="3">
+        <f t="array" ref="I76:J76">N41:O41</f>
+        <v>81</v>
+      </c>
+      <c r="J76" s="3">
+        <v>18</v>
+      </c>
+      <c r="K76" s="3">
+        <f t="shared" si="15"/>
+        <v>9</v>
+      </c>
+      <c r="L76" s="3">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="M76" s="3" t="b">
+        <f>AND(K76=G76,L76=H76)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="B77" s="23">
+        <v>5</v>
+      </c>
+      <c r="C77" s="32" t="s">
         <v>141</v>
       </c>
-      <c r="D70" s="31" t="s">
-        <v>173</v>
-      </c>
-      <c r="E70" s="31" t="s">
-        <v>192</v>
-      </c>
-      <c r="F70" s="23">
-        <v>42</v>
-      </c>
-      <c r="G70" s="23">
-        <f>SQRT(F70)</f>
-        <v>6.4807406984078604</v>
-      </c>
-      <c r="H70" s="23">
-        <f>1/2/SQRT(F70)</f>
-        <v>7.7151674981045956E-2</v>
-      </c>
-      <c r="I70" s="3">
-        <f t="array" ref="I70:J70">$G$18:$H$18</f>
-        <v>42</v>
-      </c>
-      <c r="J70" s="3">
-        <v>1</v>
-      </c>
-      <c r="K70" s="3">
-        <f t="shared" ref="K70:K72" si="10">SQRT(I70)</f>
-        <v>6.4807406984078604</v>
-      </c>
-      <c r="L70" s="3">
-        <f t="shared" ref="L70:L72" si="11">J70/2/K70</f>
-        <v>7.7151674981045956E-2</v>
-      </c>
-      <c r="M70" s="3" t="b">
-        <f>AND(K70=G70,L70=H70)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B71" s="23">
-        <v>3</v>
-      </c>
-      <c r="C71" s="32" t="s">
-        <v>164</v>
-      </c>
-      <c r="D71" s="31" t="s">
-        <v>172</v>
-      </c>
-      <c r="E71" s="31" t="s">
-        <v>196</v>
-      </c>
-      <c r="F71" s="23">
-        <v>42</v>
-      </c>
-      <c r="G71" s="23">
-        <f>SQRT(F71+24)</f>
-        <v>8.1240384046359608</v>
-      </c>
-      <c r="H71" s="23">
-        <f>1/2/SQRT(F71+24)</f>
-        <v>6.1545745489666362E-2</v>
-      </c>
-      <c r="I71" s="3">
-        <f t="array" ref="I71:J71">N26:$O$26</f>
-        <v>66</v>
-      </c>
-      <c r="J71" s="3">
-        <v>1</v>
-      </c>
-      <c r="K71" s="3">
-        <f t="shared" si="10"/>
-        <v>8.1240384046359608</v>
-      </c>
-      <c r="L71" s="3">
-        <f t="shared" si="11"/>
-        <v>6.1545745489666362E-2</v>
-      </c>
-      <c r="M71" s="3" t="b">
-        <f>AND(K71=G71,L71=H71)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B72" s="23">
-        <v>4</v>
-      </c>
-      <c r="C72" s="32" t="s">
-        <v>157</v>
-      </c>
-      <c r="D72" s="31" t="s">
-        <v>193</v>
-      </c>
-      <c r="E72" s="31" t="s">
-        <v>195</v>
-      </c>
-      <c r="F72" s="23">
-        <v>42</v>
-      </c>
-      <c r="G72" s="23">
-        <f>F72</f>
-        <v>42</v>
-      </c>
-      <c r="H72" s="23">
-        <v>1</v>
-      </c>
-      <c r="I72" s="3">
-        <f t="array" ref="I72:J72">N37:O37</f>
-        <v>1764</v>
-      </c>
-      <c r="J72" s="3">
-        <v>84</v>
-      </c>
-      <c r="K72" s="3">
-        <f t="shared" si="10"/>
-        <v>42</v>
-      </c>
-      <c r="L72" s="3">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="M72" s="3" t="b">
-        <f>AND(K72=G72,L72=H72)</f>
-        <v>1</v>
+      <c r="D77" s="31" t="s">
+        <v>161</v>
+      </c>
+      <c r="E77" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="F77" s="23">
+        <f>-X</f>
+        <v>-9</v>
+      </c>
+      <c r="G77" s="23" t="e">
+        <f>SQRT(F77)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="H77" s="23" t="e">
+        <f>1/2/SQRT(F77)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="I77" s="3">
+        <f>-X</f>
+        <v>-9</v>
+      </c>
+      <c r="J77" s="3">
+        <v>1</v>
+      </c>
+      <c r="K77" s="3" t="e">
+        <f t="shared" ref="K77" si="17">SQRT(I77)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="L77" s="3" t="e">
+        <f t="shared" ref="L77" si="18">J77/2/K77</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="M77" s="3" t="e">
+        <f>AND(K77=G77,L77=H77)</f>
+        <v>#NUM!</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3"/>
-  <conditionalFormatting sqref="P25:P27">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+  <conditionalFormatting sqref="P29:P31">
+    <cfRule type="cellIs" dxfId="15" priority="11" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="12" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P35:P39">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+  <conditionalFormatting sqref="P39:P43">
+    <cfRule type="cellIs" dxfId="13" priority="9" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="10" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M46:M47">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+  <conditionalFormatting sqref="M50:M51">
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M56:M60">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+  <conditionalFormatting sqref="M60:M65">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M69:M72">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <conditionalFormatting sqref="M73:M76">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M77">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -29889,6 +30853,66 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="19.5" thickTop="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B8" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B9" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B11" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B14" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B16" t="s">
+        <v>185</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:G64"/>
@@ -30331,7 +31355,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D25"/>
   <sheetViews>

</xml_diff>

<commit_message>
Field Scaling / test implemented
</commit_message>
<xml_diff>
--- a/10_LogicPaper_math.xlsx
+++ b/10_LogicPaper_math.xlsx
@@ -1289,107 +1289,7 @@
     <cellStyle name="標準 2" xfId="1"/>
     <cellStyle name="標準 2 2" xfId="3"/>
   </cellStyles>
-  <dxfs count="42">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="32">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1964,11 +1864,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-923425536"/>
-        <c:axId val="-923426624"/>
+        <c:axId val="1298459872"/>
+        <c:axId val="1298460960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-923425536"/>
+        <c:axId val="1298459872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2025,12 +1925,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-923426624"/>
+        <c:crossAx val="1298460960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-923426624"/>
+        <c:axId val="1298460960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2087,7 +1987,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-923425536"/>
+        <c:crossAx val="1298459872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5584,8 +5484,8 @@
       <xdr:rowOff>117231</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1354794" cy="853503"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="テキスト ボックス 2"/>
@@ -6057,7 +5957,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="テキスト ボックス 2"/>
@@ -6174,8 +6074,8 @@
       <xdr:rowOff>29308</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1413592" cy="438325"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="テキスト ボックス 3"/>
@@ -6451,7 +6351,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="テキスト ボックス 3"/>
@@ -6532,8 +6432,8 @@
       <xdr:rowOff>131885</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="832407" cy="438325"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="テキスト ボックス 4"/>
@@ -6753,7 +6653,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="テキスト ボックス 4"/>
@@ -6834,8 +6734,8 @@
       <xdr:rowOff>212481</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="696793" cy="438325"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="テキスト ボックス 5"/>
@@ -6967,7 +6867,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="テキスト ボックス 5"/>
@@ -7048,8 +6948,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1159933" cy="850682"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="テキスト ボックス 6"/>
@@ -7261,7 +7161,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="テキスト ボックス 6"/>
@@ -10810,8 +10710,8 @@
       <xdr:rowOff>58616</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2178545" cy="745717"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="テキスト ボックス 7"/>
@@ -11208,7 +11108,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="テキスト ボックス 7"/>
@@ -11320,8 +11220,8 @@
       <xdr:rowOff>131884</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2285947" cy="896143"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="テキスト ボックス 6"/>
@@ -11679,7 +11579,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="テキスト ボックス 6"/>
@@ -11804,8 +11704,8 @@
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1235658" cy="442237"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="テキスト ボックス 2"/>
@@ -12113,7 +12013,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="テキスト ボックス 2"/>
@@ -12419,8 +12319,8 @@
       <xdr:rowOff>47626</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1368457" cy="429669"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="テキスト ボックス 4"/>
@@ -12563,7 +12463,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="テキスト ボックス 4"/>
@@ -12871,8 +12771,8 @@
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="968727" cy="438325"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="テキスト ボックス 6"/>
@@ -13265,7 +13165,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="テキスト ボックス 6"/>
@@ -13405,8 +13305,8 @@
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1322990" cy="438325"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="テキスト ボックス 7"/>
@@ -13893,7 +13793,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="テキスト ボックス 7"/>
@@ -14033,8 +13933,8 @@
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="701602" cy="438325"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="テキスト ボックス 8"/>
@@ -14285,7 +14185,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="テキスト ボックス 8"/>
@@ -14425,8 +14325,8 @@
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="739818" cy="900375"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="テキスト ボックス 9"/>
@@ -14812,7 +14712,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="テキスト ボックス 9"/>
@@ -14952,8 +14852,8 @@
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="670375" cy="628249"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="テキスト ボックス 10"/>
@@ -15266,7 +15166,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="テキスト ボックス 10"/>
@@ -16187,8 +16087,8 @@
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="954236" cy="429669"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="テキスト ボックス 3"/>
@@ -16581,7 +16481,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="テキスト ボックス 3"/>
@@ -16721,8 +16621,8 @@
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1388137" cy="429669"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="テキスト ボックス 4"/>
@@ -17351,7 +17251,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="テキスト ボックス 4"/>
@@ -17507,8 +17407,8 @@
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="691151" cy="429669"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="テキスト ボックス 5"/>
@@ -17814,7 +17714,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="テキスト ボックス 5"/>
@@ -17971,8 +17871,8 @@
       <xdr:rowOff>197827</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1054583" cy="880819"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="テキスト ボックス 6"/>
@@ -18680,7 +18580,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="テキスト ボックス 6"/>
@@ -18837,8 +18737,8 @@
       <xdr:rowOff>219808</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1049583" cy="651460"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="テキスト ボックス 7"/>
@@ -19357,7 +19257,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="テキスト ボックス 7"/>
@@ -19540,8 +19440,8 @@
       <xdr:rowOff>153866</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="544060" cy="438325"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="テキスト ボックス 8"/>
@@ -19700,7 +19600,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="テキスト ボックス 8"/>
@@ -19835,8 +19735,8 @@
       <xdr:rowOff>183173</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="733662" cy="863250"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="テキスト ボックス 9"/>
@@ -20163,7 +20063,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="テキスト ボックス 9"/>
@@ -20398,8 +20298,8 @@
       <xdr:rowOff>153865</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="733662" cy="1007712"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="テキスト ボックス 10"/>
@@ -20767,7 +20667,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="テキスト ボックス 10"/>
@@ -21002,8 +20902,8 @@
       <xdr:rowOff>168519</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1284775" cy="219227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="14" name="テキスト ボックス 13"/>
@@ -21175,7 +21075,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="14" name="テキスト ボックス 13"/>
@@ -21294,8 +21194,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1172372" cy="226280"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="15" name="テキスト ボックス 14"/>
@@ -21590,7 +21490,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="15" name="テキスト ボックス 14"/>
@@ -21709,8 +21609,8 @@
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1231234" cy="226216"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="16" name="テキスト ボックス 15"/>
@@ -22050,7 +21950,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="16" name="テキスト ボックス 15"/>
@@ -22155,8 +22055,8 @@
       <xdr:rowOff>51288</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1023678" cy="1237262"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="17" name="テキスト ボックス 16"/>
@@ -22679,7 +22579,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="17" name="テキスト ボックス 16"/>
@@ -22996,8 +22896,8 @@
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1023678" cy="1214884"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="18" name="テキスト ボックス 17"/>
@@ -23520,7 +23420,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="18" name="テキスト ボックス 17"/>
@@ -39254,7 +39154,7 @@
   <dimension ref="A1:L121"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G120" sqref="G120:H120"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -39767,11 +39667,11 @@
         <v>-1</v>
       </c>
       <c r="G39" s="3">
-        <f>-C39</f>
+        <f t="shared" ref="G39:H42" si="5">-C39</f>
         <v>-1</v>
       </c>
       <c r="H39" s="3">
-        <f>-D39</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I39" s="3" t="b">
@@ -39794,15 +39694,15 @@
         <v>1.4142135623730951</v>
       </c>
       <c r="F40" s="31">
-        <f t="shared" ref="F40:F42" si="5">-E40</f>
+        <f t="shared" ref="F40:F42" si="6">-E40</f>
         <v>-1.4142135623730951</v>
       </c>
       <c r="G40" s="3">
-        <f>-C40</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H40" s="3">
-        <f>-D40</f>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
       <c r="I40" s="3" t="b">
@@ -39825,15 +39725,15 @@
         <v>1</v>
       </c>
       <c r="F41" s="31">
+        <f t="shared" si="6"/>
+        <v>-1</v>
+      </c>
+      <c r="G41" s="3">
         <f t="shared" si="5"/>
         <v>-1</v>
       </c>
-      <c r="G41" s="3">
-        <f>-C41</f>
-        <v>-1</v>
-      </c>
       <c r="H41" s="3">
-        <f>-D41</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I41" s="3" t="b">
@@ -39856,15 +39756,15 @@
         <v>2.4142135623730949</v>
       </c>
       <c r="F42" s="31">
+        <f t="shared" si="6"/>
+        <v>-2.4142135623730949</v>
+      </c>
+      <c r="G42" s="3">
         <f t="shared" si="5"/>
-        <v>-2.4142135623730949</v>
-      </c>
-      <c r="G42" s="3">
-        <f>-C42</f>
         <v>-1</v>
       </c>
       <c r="H42" s="3">
-        <f>-D42</f>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
       <c r="I42" s="3" t="b">
@@ -39954,7 +39854,7 @@
         <v>1.4142135623730951</v>
       </c>
       <c r="F55" s="31">
-        <f t="shared" ref="F55:F58" si="6">1/E55</f>
+        <f t="shared" ref="F55:F58" si="7">1/E55</f>
         <v>0.70710678118654746</v>
       </c>
       <c r="G55" s="3">
@@ -39985,7 +39885,7 @@
         <v>1</v>
       </c>
       <c r="F56" s="31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="G56" s="3">
@@ -40016,7 +39916,7 @@
         <v>2.4142135623730949</v>
       </c>
       <c r="F57" s="31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.41421356237309509</v>
       </c>
       <c r="G57" s="3">
@@ -40047,7 +39947,7 @@
         <v>0</v>
       </c>
       <c r="F58" s="31" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G58" s="3" t="e">
@@ -40195,7 +40095,7 @@
         <v>0</v>
       </c>
       <c r="E112" s="31">
-        <f>C112+SQRT(R_)*D112</f>
+        <f t="shared" ref="E112:E121" si="8">C112+SQRT(R_)*D112</f>
         <v>-42</v>
       </c>
       <c r="F112" s="31" t="e">
@@ -40211,7 +40111,7 @@
         <v>#N/A</v>
       </c>
       <c r="I112" s="3" t="e">
-        <f>ABS(G112+SQRT(R_)*H112-F112)&lt;0.0000000001</f>
+        <f t="shared" ref="I112:I121" si="9">ABS(G112+SQRT(R_)*H112-F112)&lt;0.0000000001</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -40226,11 +40126,11 @@
         <v>0</v>
       </c>
       <c r="E113" s="31">
-        <f>C113+SQRT(R_)*D113</f>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="F113" s="31">
-        <f t="shared" ref="F113:F121" si="7">SQRT(E113)</f>
+        <f t="shared" ref="F113:F121" si="10">SQRT(E113)</f>
         <v>1.7320508075688772</v>
       </c>
       <c r="G113" s="3" t="e">
@@ -40242,7 +40142,7 @@
         <v>#N/A</v>
       </c>
       <c r="I113" s="3" t="e">
-        <f>ABS(G113+SQRT(R_)*H113-F113)&lt;0.0000000001</f>
+        <f t="shared" si="9"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -40257,11 +40157,11 @@
         <v>0</v>
       </c>
       <c r="E114" s="31">
-        <f>C114+SQRT(R_)*D114</f>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="F114" s="31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="G114" s="3">
@@ -40272,7 +40172,7 @@
         <v>0</v>
       </c>
       <c r="I114" s="3" t="b">
-        <f>ABS(G114+SQRT(R_)*H114-F114)&lt;0.0000000001</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -40287,22 +40187,22 @@
         <v>0</v>
       </c>
       <c r="E115" s="31">
-        <f>C115+SQRT(R_)*D115</f>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="F115" s="31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>4.2426406871192848</v>
       </c>
       <c r="G115" s="3">
         <v>0</v>
       </c>
       <c r="H115" s="3">
-        <f>SQRT(C115/2)</f>
+        <f>SQRT(C115/R_)</f>
         <v>3</v>
       </c>
       <c r="I115" s="3" t="b">
-        <f>ABS(G115+SQRT(R_)*H115-F115)&lt;0.0000000001</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -40317,11 +40217,11 @@
         <v>3</v>
       </c>
       <c r="E116" s="31">
-        <f>C116+SQRT(R_)*D116</f>
+        <f t="shared" si="8"/>
         <v>6.2426406871192857</v>
       </c>
       <c r="F116" s="31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>2.4985277038926914</v>
       </c>
       <c r="G116" s="3" t="e">
@@ -40333,7 +40233,7 @@
         <v>#N/A</v>
       </c>
       <c r="I116" s="3" t="e">
-        <f>ABS(G116+SQRT(R_)*H116-F116)&lt;0.0000000001</f>
+        <f t="shared" si="9"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -40348,11 +40248,11 @@
         <v>2</v>
       </c>
       <c r="E117" s="31">
-        <f>C117+SQRT(R_)*D117</f>
+        <f t="shared" si="8"/>
         <v>5.8284271247461898</v>
       </c>
       <c r="F117" s="31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>2.4142135623730949</v>
       </c>
       <c r="G117" s="3">
@@ -40364,7 +40264,7 @@
         <v>1</v>
       </c>
       <c r="I117" s="3" t="b">
-        <f>ABS(G117+SQRT(R_)*H117-F117)&lt;0.0000000001</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -40379,11 +40279,11 @@
         <v>12</v>
       </c>
       <c r="E118" s="31">
-        <f>C118+SQRT(R_)*D118</f>
+        <f t="shared" si="8"/>
         <v>33.970562748477143</v>
       </c>
       <c r="F118" s="31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>5.8284271247461898</v>
       </c>
       <c r="G118" s="3">
@@ -40395,7 +40295,7 @@
         <v>2</v>
       </c>
       <c r="I118" s="3" t="b">
-        <f>ABS(G118+SQRT(R_)*H118-F118)&lt;0.0000000001</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -40410,11 +40310,11 @@
         <v>5</v>
       </c>
       <c r="E119" s="31">
-        <f>C119+SQRT(R_)*D119</f>
+        <f t="shared" si="8"/>
         <v>19.071067811865476</v>
       </c>
       <c r="F119" s="31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>4.3670433718782178</v>
       </c>
       <c r="G119" s="3" t="e">
@@ -40426,7 +40326,7 @@
         <v>#N/A</v>
       </c>
       <c r="I119" s="3" t="e">
-        <f>ABS(G119+SQRT(R_)*H119-F119)&lt;0.0000000001</f>
+        <f t="shared" si="9"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -40441,11 +40341,11 @@
         <v>6</v>
       </c>
       <c r="E120" s="31">
-        <f>C120+SQRT(R_)*D120</f>
+        <f t="shared" si="8"/>
         <v>17.485281374238571</v>
       </c>
       <c r="F120" s="31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>4.1815405503520555</v>
       </c>
       <c r="G120" s="3" t="e">
@@ -40457,7 +40357,7 @@
         <v>#N/A</v>
       </c>
       <c r="I120" s="3" t="e">
-        <f>ABS(G120+SQRT(R_)*H120-F120)&lt;0.0000000001</f>
+        <f t="shared" si="9"/>
         <v>#N/A</v>
       </c>
     </row>
@@ -40472,11 +40372,11 @@
         <v>0</v>
       </c>
       <c r="E121" s="31">
-        <f>C121+SQRT(R_)*D121</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F121" s="31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="G121" s="3">
@@ -40486,7 +40386,7 @@
         <v>0</v>
       </c>
       <c r="I121" s="3" t="b">
-        <f>ABS(G121+SQRT(R_)*H121-F121)&lt;0.0000000001</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>